<commit_message>
Reading again after bugfix (IC49 different)
</commit_message>
<xml_diff>
--- a/reads/reads.xlsx
+++ b/reads/reads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PalAnalyzer\reads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A094669-D415-49A5-ACB3-82AACF52FEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8781FC6F-6C67-48A5-AD14-59C0A914AD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="57">
   <si>
     <t>Ref</t>
   </si>
@@ -159,9 +159,6 @@
     <t>I/O mask / Outputs</t>
   </si>
   <si>
-    <t>Yes (if IC socketed)</t>
-  </si>
-  <si>
     <t>Inputs 16R4</t>
   </si>
   <si>
@@ -193,13 +190,19 @@
   </si>
   <si>
     <t xml:space="preserve">IC7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +214,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -353,6 +363,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +647,7 @@
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +715,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -713,16 +724,16 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
         <v>49</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>9</v>
@@ -774,10 +785,10 @@
         <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>9</v>
@@ -832,6 +843,9 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
@@ -888,11 +902,11 @@
       <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>41</v>
@@ -939,10 +953,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
         <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>9</v>
@@ -989,7 +1003,7 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>9</v>
@@ -1033,7 +1047,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
         <v>42</v>
@@ -1124,7 +1138,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G11" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>9</v>
@@ -1174,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>10</v>
@@ -1211,10 +1225,10 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -1230,10 +1244,10 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>9</v>

</xml_diff>